<commit_message>
remove images and update readme
</commit_message>
<xml_diff>
--- a/data/processed/df.xlsx
+++ b/data/processed/df.xlsx
@@ -460,10 +460,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>15613.2626953125</v>
+        <v>15309.44921875</v>
       </c>
       <c r="C2" t="n">
-        <v>15596.736328125</v>
+        <v>15302.58203125</v>
       </c>
       <c r="D2" t="n">
         <v>15616</v>
@@ -474,10 +474,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>15185.23046875</v>
+        <v>14884.005859375</v>
       </c>
       <c r="C3" t="n">
-        <v>15045.4326171875</v>
+        <v>14794.0947265625</v>
       </c>
       <c r="D3" t="n">
         <v>15476</v>
@@ -488,10 +488,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>15036.2607421875</v>
+        <v>14768.142578125</v>
       </c>
       <c r="C4" t="n">
-        <v>14420.3046875</v>
+        <v>14540.65234375</v>
       </c>
       <c r="D4" t="n">
         <v>14665</v>
@@ -502,10 +502,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>13748.802734375</v>
+        <v>13538.70703125</v>
       </c>
       <c r="C5" t="n">
-        <v>13593.16796875</v>
+        <v>13830.166015625</v>
       </c>
       <c r="D5" t="n">
         <v>13680</v>
@@ -516,10 +516,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>12943.6328125</v>
+        <v>12859.1103515625</v>
       </c>
       <c r="C6" t="n">
-        <v>12940.1845703125</v>
+        <v>13013.0673828125</v>
       </c>
       <c r="D6" t="n">
         <v>12927</v>
@@ -530,10 +530,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>12439.3681640625</v>
+        <v>12269.5048828125</v>
       </c>
       <c r="C7" t="n">
-        <v>12412.9208984375</v>
+        <v>12371.6123046875</v>
       </c>
       <c r="D7" t="n">
         <v>12397</v>
@@ -544,10 +544,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>12058.423828125</v>
+        <v>11926.3623046875</v>
       </c>
       <c r="C8" t="n">
-        <v>12000.2216796875</v>
+        <v>12090.4033203125</v>
       </c>
       <c r="D8" t="n">
         <v>12096</v>
@@ -558,10 +558,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>12053.1728515625</v>
+        <v>12001.630859375</v>
       </c>
       <c r="C9" t="n">
-        <v>11708.1865234375</v>
+        <v>12138.8408203125</v>
       </c>
       <c r="D9" t="n">
         <v>11938</v>
@@ -572,10 +572,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>12229.2294921875</v>
+        <v>12175.1884765625</v>
       </c>
       <c r="C10" t="n">
-        <v>11911.9296875</v>
+        <v>12307.7802734375</v>
       </c>
       <c r="D10" t="n">
         <v>12109</v>
@@ -586,10 +586,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>12712.23046875</v>
+        <v>12608.7919921875</v>
       </c>
       <c r="C11" t="n">
-        <v>12615.939453125</v>
+        <v>12608.69921875</v>
       </c>
       <c r="D11" t="n">
         <v>12559</v>
@@ -600,10 +600,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>13324.6396484375</v>
+        <v>13181.7724609375</v>
       </c>
       <c r="C12" t="n">
-        <v>13451.533203125</v>
+        <v>13094.1015625</v>
       </c>
       <c r="D12" t="n">
         <v>13473.9990234375</v>
@@ -614,10 +614,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>14396.8779296875</v>
+        <v>14199.2421875</v>
       </c>
       <c r="C13" t="n">
-        <v>14186.982421875</v>
+        <v>13948.109375</v>
       </c>
       <c r="D13" t="n">
         <v>14033</v>
@@ -628,10 +628,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>14688.48828125</v>
+        <v>14466.3671875</v>
       </c>
       <c r="C14" t="n">
-        <v>14881.283203125</v>
+        <v>14621.91015625</v>
       </c>
       <c r="D14" t="n">
         <v>14623</v>
@@ -642,10 +642,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>15195.9189453125</v>
+        <v>14994.5361328125</v>
       </c>
       <c r="C15" t="n">
-        <v>15479.8408203125</v>
+        <v>15063.03125</v>
       </c>
       <c r="D15" t="n">
         <v>15168</v>
@@ -656,10 +656,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>15645.9482421875</v>
+        <v>15449.3779296875</v>
       </c>
       <c r="C16" t="n">
-        <v>15957.822265625</v>
+        <v>15427.765625</v>
       </c>
       <c r="D16" t="n">
         <v>15872</v>
@@ -670,10 +670,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>16379.4853515625</v>
+        <v>16157.73828125</v>
       </c>
       <c r="C17" t="n">
-        <v>16396.220703125</v>
+        <v>15959.0390625</v>
       </c>
       <c r="D17" t="n">
         <v>16352.9990234375</v>
@@ -684,10 +684,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>16679.248046875</v>
+        <v>16467.64453125</v>
       </c>
       <c r="C18" t="n">
-        <v>16739.9765625</v>
+        <v>16412.861328125</v>
       </c>
       <c r="D18" t="n">
         <v>17001</v>
@@ -698,10 +698,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>17404.123046875</v>
+        <v>17199.10546875</v>
       </c>
       <c r="C19" t="n">
-        <v>17247.927734375</v>
+        <v>16931.021484375</v>
       </c>
       <c r="D19" t="n">
         <v>17582</v>
@@ -712,10 +712,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>17894.123046875</v>
+        <v>17669.318359375</v>
       </c>
       <c r="C20" t="n">
-        <v>17753.91015625</v>
+        <v>17469.56640625</v>
       </c>
       <c r="D20" t="n">
         <v>17889</v>
@@ -726,10 +726,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>18029.642578125</v>
+        <v>17784.96875</v>
       </c>
       <c r="C21" t="n">
-        <v>18109.990234375</v>
+        <v>17735.212890625</v>
       </c>
       <c r="D21" t="n">
         <v>18176</v>
@@ -740,10 +740,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>18308.341796875</v>
+        <v>18067.65234375</v>
       </c>
       <c r="C22" t="n">
-        <v>18308.642578125</v>
+        <v>17861.19140625</v>
       </c>
       <c r="D22" t="n">
         <v>18262</v>
@@ -754,10 +754,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>18239.55859375</v>
+        <v>17953.484375</v>
       </c>
       <c r="C23" t="n">
-        <v>18302.05078125</v>
+        <v>17835.322265625</v>
       </c>
       <c r="D23" t="n">
         <v>18174.001953125</v>
@@ -768,10 +768,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>18018.42578125</v>
+        <v>17743.22265625</v>
       </c>
       <c r="C24" t="n">
-        <v>18073.533203125</v>
+        <v>17610.302734375</v>
       </c>
       <c r="D24" t="n">
         <v>17875</v>
@@ -782,10 +782,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>17539.169921875</v>
+        <v>17284.7421875</v>
       </c>
       <c r="C25" t="n">
-        <v>17615.662109375</v>
+        <v>17173.865234375</v>
       </c>
       <c r="D25" t="n">
         <v>17307</v>
@@ -796,10 +796,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>16758.03125</v>
+        <v>16520.587890625</v>
       </c>
       <c r="C26" t="n">
-        <v>16918.75</v>
+        <v>16488.74609375</v>
       </c>
       <c r="D26" t="n">
         <v>17022</v>
@@ -810,10 +810,10 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>16532.701171875</v>
+        <v>16365.666015625</v>
       </c>
       <c r="C27" t="n">
-        <v>16189.0546875</v>
+        <v>16004.28515625</v>
       </c>
       <c r="D27" t="n">
         <v>16725</v>
@@ -824,10 +824,10 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>16030.70703125</v>
+        <v>15898.8076171875</v>
       </c>
       <c r="C28" t="n">
-        <v>15444.9794921875</v>
+        <v>15656.7021484375</v>
       </c>
       <c r="D28" t="n">
         <v>15591.9990234375</v>
@@ -838,10 +838,10 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>14353.1875</v>
+        <v>14290.2900390625</v>
       </c>
       <c r="C29" t="n">
-        <v>14458.9619140625</v>
+        <v>14627.13671875</v>
       </c>
       <c r="D29" t="n">
         <v>14363</v>
@@ -852,10 +852,10 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>13436.681640625</v>
+        <v>13360.5302734375</v>
       </c>
       <c r="C30" t="n">
-        <v>13500.6669921875</v>
+        <v>13508.5732421875</v>
       </c>
       <c r="D30" t="n">
         <v>13501</v>
@@ -866,10 +866,10 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>12915.2470703125</v>
+        <v>12814.4111328125</v>
       </c>
       <c r="C31" t="n">
-        <v>12836.6298828125</v>
+        <v>12794.5791015625</v>
       </c>
       <c r="D31" t="n">
         <v>12787</v>
@@ -880,10 +880,10 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>12362.6533203125</v>
+        <v>12220.5966796875</v>
       </c>
       <c r="C32" t="n">
-        <v>12411.2177734375</v>
+        <v>12438.80078125</v>
       </c>
       <c r="D32" t="n">
         <v>12382</v>
@@ -894,10 +894,10 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>12286.7451171875</v>
+        <v>12137.9599609375</v>
       </c>
       <c r="C33" t="n">
-        <v>12082.0693359375</v>
+        <v>12415.9873046875</v>
       </c>
       <c r="D33" t="n">
         <v>12275</v>
@@ -908,10 +908,10 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>12567.09765625</v>
+        <v>12481.8505859375</v>
       </c>
       <c r="C34" t="n">
-        <v>12242.0068359375</v>
+        <v>12636.30859375</v>
       </c>
       <c r="D34" t="n">
         <v>12498</v>
@@ -922,10 +922,10 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>13093.6279296875</v>
+        <v>13028.03515625</v>
       </c>
       <c r="C35" t="n">
-        <v>12978.498046875</v>
+        <v>13052.232421875</v>
       </c>
       <c r="D35" t="n">
         <v>12926</v>
@@ -936,10 +936,10 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>13678.6572265625</v>
+        <v>13578.73828125</v>
       </c>
       <c r="C36" t="n">
-        <v>13808.9716796875</v>
+        <v>13576.318359375</v>
       </c>
       <c r="D36" t="n">
         <v>13871</v>
@@ -950,10 +950,10 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>14829.248046875</v>
+        <v>14667.8779296875</v>
       </c>
       <c r="C37" t="n">
-        <v>14570.94921875</v>
+        <v>14437.9091796875</v>
       </c>
       <c r="D37" t="n">
         <v>14554</v>
@@ -964,10 +964,10 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>15287.142578125</v>
+        <v>15072.005859375</v>
       </c>
       <c r="C38" t="n">
-        <v>15337.0712890625</v>
+        <v>15187.740234375</v>
       </c>
       <c r="D38" t="n">
         <v>15071.9990234375</v>
@@ -978,10 +978,10 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>15617.7333984375</v>
+        <v>15405.0126953125</v>
       </c>
       <c r="C39" t="n">
-        <v>15947.099609375</v>
+        <v>15582.5771484375</v>
       </c>
       <c r="D39" t="n">
         <v>15480</v>
@@ -992,10 +992,10 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>15894.3232421875</v>
+        <v>15702.408203125</v>
       </c>
       <c r="C40" t="n">
-        <v>16330.25390625</v>
+        <v>15764.1669921875</v>
       </c>
       <c r="D40" t="n">
         <v>15975</v>
@@ -1006,10 +1006,10 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>16385.439453125</v>
+        <v>16175.1669921875</v>
       </c>
       <c r="C41" t="n">
-        <v>16558.28125</v>
+        <v>16043.0771484375</v>
       </c>
       <c r="D41" t="n">
         <v>16157</v>
@@ -1020,10 +1020,10 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>16347.4921875</v>
+        <v>16147.7255859375</v>
       </c>
       <c r="C42" t="n">
-        <v>16660.7265625</v>
+        <v>16182.9326171875</v>
       </c>
       <c r="D42" t="n">
         <v>16566</v>
@@ -1034,10 +1034,10 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>16883.1484375</v>
+        <v>16707.806640625</v>
       </c>
       <c r="C43" t="n">
-        <v>16870.033203125</v>
+        <v>16445.6953125</v>
       </c>
       <c r="D43" t="n">
         <v>16881.998046875</v>
@@ -1048,10 +1048,10 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>17100.2421875</v>
+        <v>16907.0546875</v>
       </c>
       <c r="C44" t="n">
-        <v>17078.056640625</v>
+        <v>16767.56640625</v>
       </c>
       <c r="D44" t="n">
         <v>16984</v>
@@ -1062,10 +1062,10 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>17080.3828125</v>
+        <v>16881.302734375</v>
       </c>
       <c r="C45" t="n">
-        <v>17210.455078125</v>
+        <v>16870.74609375</v>
       </c>
       <c r="D45" t="n">
         <v>16779.998046875</v>
@@ -1076,10 +1076,10 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>16710.791015625</v>
+        <v>16523.4140625</v>
       </c>
       <c r="C46" t="n">
-        <v>17133.01953125</v>
+        <v>16602.150390625</v>
       </c>
       <c r="D46" t="n">
         <v>16687</v>
@@ -1090,10 +1090,10 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>16685.767578125</v>
+        <v>16474.478515625</v>
       </c>
       <c r="C47" t="n">
-        <v>16912.39453125</v>
+        <v>16334.7236328125</v>
       </c>
       <c r="D47" t="n">
         <v>16874</v>
@@ -1104,10 +1104,10 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>16955.509765625</v>
+        <v>16711.22265625</v>
       </c>
       <c r="C48" t="n">
-        <v>16721.8046875</v>
+        <v>16392.23828125</v>
       </c>
       <c r="D48" t="n">
         <v>16727</v>
@@ -1118,10 +1118,10 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>16504.470703125</v>
+        <v>16275.908203125</v>
       </c>
       <c r="C49" t="n">
-        <v>16450.740234375</v>
+        <v>16264.2197265625</v>
       </c>
       <c r="D49" t="n">
         <v>16674</v>
@@ -1132,10 +1132,10 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>16446.609375</v>
+        <v>16309.34375</v>
       </c>
       <c r="C50" t="n">
-        <v>16144.87890625</v>
+        <v>16045.505859375</v>
       </c>
       <c r="D50" t="n">
         <v>16556</v>
@@ -1146,10 +1146,10 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>16159.134765625</v>
+        <v>16042.373046875</v>
       </c>
       <c r="C51" t="n">
-        <v>15765.396484375</v>
+        <v>15820.392578125</v>
       </c>
       <c r="D51" t="n">
         <v>16252</v>
@@ -1160,10 +1160,10 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>15635.3203125</v>
+        <v>15565.4931640625</v>
       </c>
       <c r="C52" t="n">
-        <v>15203.4384765625</v>
+        <v>15421.640625</v>
       </c>
       <c r="D52" t="n">
         <v>15504</v>
@@ -1174,10 +1174,10 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>14568.126953125</v>
+        <v>14542.8525390625</v>
       </c>
       <c r="C53" t="n">
-        <v>14387.0146484375</v>
+        <v>14595.0224609375</v>
       </c>
       <c r="D53" t="n">
         <v>14424</v>
@@ -1188,10 +1188,10 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>13687.7900390625</v>
+        <v>13323.4716796875</v>
       </c>
       <c r="C54" t="n">
-        <v>13543.7626953125</v>
+        <v>13655.8388671875</v>
       </c>
       <c r="D54" t="n">
         <v>13538</v>
@@ -1202,10 +1202,10 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>13095.09765625</v>
+        <v>12919.025390625</v>
       </c>
       <c r="C55" t="n">
-        <v>12908.2587890625</v>
+        <v>12838.3134765625</v>
       </c>
       <c r="D55" t="n">
         <v>12903</v>
@@ -1216,10 +1216,10 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>12619.908203125</v>
+        <v>12366.013671875</v>
       </c>
       <c r="C56" t="n">
-        <v>12462.935546875</v>
+        <v>12429.8125</v>
       </c>
       <c r="D56" t="n">
         <v>12506</v>
@@ -1230,10 +1230,10 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>12473.7109375</v>
+        <v>12220.0439453125</v>
       </c>
       <c r="C57" t="n">
-        <v>12164.1640625</v>
+        <v>12411.171875</v>
       </c>
       <c r="D57" t="n">
         <v>12205.9990234375</v>
@@ -1244,10 +1244,10 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>12436.2275390625</v>
+        <v>12272.83203125</v>
       </c>
       <c r="C58" t="n">
-        <v>12188.5126953125</v>
+        <v>12497.9267578125</v>
       </c>
       <c r="D58" t="n">
         <v>12295</v>
@@ -1258,10 +1258,10 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>12822.994140625</v>
+        <v>12706.513671875</v>
       </c>
       <c r="C59" t="n">
-        <v>12797.9765625</v>
+        <v>12739.5986328125</v>
       </c>
       <c r="D59" t="n">
         <v>12714</v>
@@ -1272,10 +1272,10 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>13448.7861328125</v>
+        <v>13308.158203125</v>
       </c>
       <c r="C60" t="n">
-        <v>13517.115234375</v>
+        <v>13224.740234375</v>
       </c>
       <c r="D60" t="n">
         <v>13511.9990234375</v>
@@ -1286,10 +1286,10 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>14393.4609375</v>
+        <v>14209.0966796875</v>
       </c>
       <c r="C61" t="n">
-        <v>14178.201171875</v>
+        <v>14032.8544921875</v>
       </c>
       <c r="D61" t="n">
         <v>14139</v>
@@ -1300,10 +1300,10 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>14858.591796875</v>
+        <v>14645.0732421875</v>
       </c>
       <c r="C62" t="n">
-        <v>14854.36328125</v>
+        <v>14745.5380859375</v>
       </c>
       <c r="D62" t="n">
         <v>14684.9990234375</v>
@@ -1314,10 +1314,10 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>15280.20703125</v>
+        <v>15061.591796875</v>
       </c>
       <c r="C63" t="n">
-        <v>15425.2275390625</v>
+        <v>15191.1611328125</v>
       </c>
       <c r="D63" t="n">
         <v>15223</v>
@@ -1328,10 +1328,10 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>15745.52734375</v>
+        <v>15523.5927734375</v>
       </c>
       <c r="C64" t="n">
-        <v>15854.22265625</v>
+        <v>15531.5126953125</v>
       </c>
       <c r="D64" t="n">
         <v>15648</v>
@@ -1342,10 +1342,10 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>16055.38671875</v>
+        <v>15813.302734375</v>
       </c>
       <c r="C65" t="n">
-        <v>16124.1064453125</v>
+        <v>15811.1455078125</v>
       </c>
       <c r="D65" t="n">
         <v>16116</v>
@@ -1356,10 +1356,10 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>16508.318359375</v>
+        <v>16275.3681640625</v>
       </c>
       <c r="C66" t="n">
-        <v>16327.4794921875</v>
+        <v>16140.1015625</v>
       </c>
       <c r="D66" t="n">
         <v>16623</v>
@@ -1370,10 +1370,10 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>16999.3984375</v>
+        <v>16761.080078125</v>
       </c>
       <c r="C67" t="n">
-        <v>16706.849609375</v>
+        <v>16575.341796875</v>
       </c>
       <c r="D67" t="n">
         <v>17007.998046875</v>
@@ -1384,10 +1384,10 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>17288.0390625</v>
+        <v>17039.498046875</v>
       </c>
       <c r="C68" t="n">
-        <v>17071.05859375</v>
+        <v>16950.1015625</v>
       </c>
       <c r="D68" t="n">
         <v>17146</v>
@@ -1398,10 +1398,10 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>17282.802734375</v>
+        <v>17033.767578125</v>
       </c>
       <c r="C69" t="n">
-        <v>17317.642578125</v>
+        <v>17052.845703125</v>
       </c>
       <c r="D69" t="n">
         <v>17193</v>
@@ -1412,10 +1412,10 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>17286.791015625</v>
+        <v>17021.45703125</v>
       </c>
       <c r="C70" t="n">
-        <v>17406.4453125</v>
+        <v>16982.546875</v>
       </c>
       <c r="D70" t="n">
         <v>17183</v>
@@ -1426,10 +1426,10 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>17219.96484375</v>
+        <v>16921.580078125</v>
       </c>
       <c r="C71" t="n">
-        <v>17338.0703125</v>
+        <v>16859.794921875</v>
       </c>
       <c r="D71" t="n">
         <v>17204</v>
@@ -1440,10 +1440,10 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>17196.19921875</v>
+        <v>16900.0234375</v>
       </c>
       <c r="C72" t="n">
-        <v>17168.640625</v>
+        <v>16767.224609375</v>
       </c>
       <c r="D72" t="n">
         <v>16870</v>
@@ -1454,10 +1454,10 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>16583.23828125</v>
+        <v>16301.7314453125</v>
       </c>
       <c r="C73" t="n">
-        <v>16791.298828125</v>
+        <v>16391.3671875</v>
       </c>
       <c r="D73" t="n">
         <v>16579</v>
@@ -1468,10 +1468,10 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>16268.3994140625</v>
+        <v>16043.4462890625</v>
       </c>
       <c r="C74" t="n">
-        <v>16282.1630859375</v>
+        <v>15936.6806640625</v>
       </c>
       <c r="D74" t="n">
         <v>16456.998046875</v>
@@ -1482,10 +1482,10 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>16096.373046875</v>
+        <v>15906.072265625</v>
       </c>
       <c r="C75" t="n">
-        <v>15789.53515625</v>
+        <v>15684.7861328125</v>
       </c>
       <c r="D75" t="n">
         <v>16197</v>
@@ -1496,10 +1496,10 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>15598.1904296875</v>
+        <v>15463.123046875</v>
       </c>
       <c r="C76" t="n">
-        <v>15208.26171875</v>
+        <v>15386.953125</v>
       </c>
       <c r="D76" t="n">
         <v>15259</v>
@@ -1510,10 +1510,10 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>14215.3857421875</v>
+        <v>14154.21484375</v>
       </c>
       <c r="C77" t="n">
-        <v>14314.8935546875</v>
+        <v>14465.091796875</v>
       </c>
       <c r="D77" t="n">
         <v>14125</v>
@@ -1524,10 +1524,10 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>13291.6337890625</v>
+        <v>13147.7841796875</v>
       </c>
       <c r="C78" t="n">
-        <v>13410.0419921875</v>
+        <v>13431.837890625</v>
       </c>
       <c r="D78" t="n">
         <v>13286</v>
@@ -1538,10 +1538,10 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>12758.564453125</v>
+        <v>12596.3232421875</v>
       </c>
       <c r="C79" t="n">
-        <v>12740.7685546875</v>
+        <v>12672.2685546875</v>
       </c>
       <c r="D79" t="n">
         <v>12587</v>
@@ -1552,10 +1552,10 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>12165.341796875</v>
+        <v>11986.1181640625</v>
       </c>
       <c r="C80" t="n">
-        <v>12288.9931640625</v>
+        <v>12216.478515625</v>
       </c>
       <c r="D80" t="n">
         <v>12296</v>
@@ -1566,10 +1566,10 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>12185.7451171875</v>
+        <v>11993.59375</v>
       </c>
       <c r="C81" t="n">
-        <v>11939.6201171875</v>
+        <v>12190.916015625</v>
       </c>
       <c r="D81" t="n">
         <v>12059</v>
@@ -1580,10 +1580,10 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>12199.1025390625</v>
+        <v>12077.7255859375</v>
       </c>
       <c r="C82" t="n">
-        <v>11896.9736328125</v>
+        <v>12320.669921875</v>
       </c>
       <c r="D82" t="n">
         <v>12224</v>
@@ -1594,10 +1594,10 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>12682.994140625</v>
+        <v>12603.6435546875</v>
       </c>
       <c r="C83" t="n">
-        <v>12512.5615234375</v>
+        <v>12637.25390625</v>
       </c>
       <c r="D83" t="n">
         <v>12781</v>
@@ -1608,10 +1608,10 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>13488.4345703125</v>
+        <v>13373.482421875</v>
       </c>
       <c r="C84" t="n">
-        <v>13371.521484375</v>
+        <v>13255.783203125</v>
       </c>
       <c r="D84" t="n">
         <v>13661</v>
@@ -1622,10 +1622,10 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>14498.0439453125</v>
+        <v>14331.125</v>
       </c>
       <c r="C85" t="n">
-        <v>14190.220703125</v>
+        <v>14178.8056640625</v>
       </c>
       <c r="D85" t="n">
         <v>14326</v>
@@ -1636,10 +1636,10 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>14978.5654296875</v>
+        <v>14777.9775390625</v>
       </c>
       <c r="C86" t="n">
-        <v>15005.388671875</v>
+        <v>14928.783203125</v>
       </c>
       <c r="D86" t="n">
         <v>14834</v>
@@ -1650,10 +1650,10 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>15327.7646484375</v>
+        <v>15116.654296875</v>
       </c>
       <c r="C87" t="n">
-        <v>15641.5625</v>
+        <v>15315.4833984375</v>
       </c>
       <c r="D87" t="n">
         <v>15309</v>
@@ -1664,10 +1664,10 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>15725.978515625</v>
+        <v>15507.1025390625</v>
       </c>
       <c r="C88" t="n">
-        <v>16041.625</v>
+        <v>15558.4296875</v>
       </c>
       <c r="D88" t="n">
         <v>16025</v>
@@ -1678,10 +1678,10 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>16515.96484375</v>
+        <v>16269.2421875</v>
       </c>
       <c r="C89" t="n">
-        <v>16366.5537109375</v>
+        <v>16058.67578125</v>
       </c>
       <c r="D89" t="n">
         <v>16651</v>
@@ -1692,10 +1692,10 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>17025.001953125</v>
+        <v>16776.046875</v>
       </c>
       <c r="C90" t="n">
-        <v>16703.7421875</v>
+        <v>16660.869140625</v>
       </c>
       <c r="D90" t="n">
         <v>17423</v>
@@ -1706,10 +1706,10 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>17855.447265625</v>
+        <v>17613.888671875</v>
       </c>
       <c r="C91" t="n">
-        <v>17293.98828125</v>
+        <v>17372.96875</v>
       </c>
       <c r="D91" t="n">
         <v>18067</v>
@@ -1720,10 +1720,10 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>18385.654296875</v>
+        <v>18133.810546875</v>
       </c>
       <c r="C92" t="n">
-        <v>17915.658203125</v>
+        <v>18018.6796875</v>
       </c>
       <c r="D92" t="n">
         <v>18534</v>
@@ -1734,10 +1734,10 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>18758.265625</v>
+        <v>18474.994140625</v>
       </c>
       <c r="C93" t="n">
-        <v>18459.11328125</v>
+        <v>18429.6953125</v>
       </c>
       <c r="D93" t="n">
         <v>18826</v>
@@ -1748,10 +1748,10 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>18956.2890625</v>
+        <v>18649.736328125</v>
       </c>
       <c r="C94" t="n">
-        <v>18824.373046875</v>
+        <v>18601.75390625</v>
       </c>
       <c r="D94" t="n">
         <v>18869</v>
@@ -1762,10 +1762,10 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>18849.060546875</v>
+        <v>18502.5234375</v>
       </c>
       <c r="C95" t="n">
-        <v>18916.115234375</v>
+        <v>18512.81640625</v>
       </c>
       <c r="D95" t="n">
         <v>18562</v>
@@ -1776,10 +1776,10 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>18329.158203125</v>
+        <v>17970.1796875</v>
       </c>
       <c r="C96" t="n">
-        <v>18638.32421875</v>
+        <v>18069.619140625</v>
       </c>
       <c r="D96" t="n">
         <v>18118</v>
@@ -1790,10 +1790,10 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>17792.24609375</v>
+        <v>17430.943359375</v>
       </c>
       <c r="C97" t="n">
-        <v>18040.521484375</v>
+        <v>17451.5546875</v>
       </c>
       <c r="D97" t="n">
         <v>17673.001953125</v>
@@ -1804,10 +1804,10 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>17262.681640625</v>
+        <v>16901.16796875</v>
       </c>
       <c r="C98" t="n">
-        <v>17280.298828125</v>
+        <v>16870.142578125</v>
       </c>
       <c r="D98" t="n">
         <v>17303</v>
@@ -1818,10 +1818,10 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>16809.125</v>
+        <v>16484.77734375</v>
       </c>
       <c r="C99" t="n">
-        <v>16539.115234375</v>
+        <v>16403.740234375</v>
       </c>
       <c r="D99" t="n">
         <v>17001</v>
@@ -1832,10 +1832,10 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>16386.5625</v>
+        <v>16145.9931640625</v>
       </c>
       <c r="C100" t="n">
-        <v>15874.0048828125</v>
+        <v>16031.2509765625</v>
       </c>
       <c r="D100" t="n">
         <v>15964</v>
@@ -1846,10 +1846,10 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>14816.4306640625</v>
+        <v>14651.4775390625</v>
       </c>
       <c r="C101" t="n">
-        <v>14917.1357421875</v>
+        <v>15071.205078125</v>
       </c>
       <c r="D101" t="n">
         <v>14809</v>

</xml_diff>